<commit_message>
Added lots of changes, including timers limiting the players and judge's time, and music/recorded audio to enhance the game experience
</commit_message>
<xml_diff>
--- a/public/mangos_game/Assets.xlsx
+++ b/public/mangos_game/Assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\CS5\git repository\public\mangos_game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0ED34A-5E34-4A81-A8CF-7564A579AF6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C5B550-0AFE-4C6B-BB16-E36582C0427B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7E3EC852-6885-4E01-BA36-ECA6C0A8927D}"/>
+    <workbookView xWindow="340" yWindow="1410" windowWidth="14400" windowHeight="7360" xr2:uid="{7E3EC852-6885-4E01-BA36-ECA6C0A8927D}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Asset Name</t>
   </si>
@@ -79,6 +79,30 @@
   </si>
   <si>
     <t>https://www.fesliyanstudios.com/royalty-free-sound-effects-download/clock-ticking-46 (Clock-Ticking-C-www.fesliyanstudios.com)</t>
+  </si>
+  <si>
+    <t>wav</t>
+  </si>
+  <si>
+    <t>mixkit-game-show-happy-timer-666</t>
+  </si>
+  <si>
+    <t>Background Game show timer</t>
+  </si>
+  <si>
+    <t>https://mixkit.co/free-sound-effects/game-show/</t>
+  </si>
+  <si>
+    <t>mixkit-game-show-suspense-waiting-667</t>
+  </si>
+  <si>
+    <t>Good-Morning-Doctor-Weird</t>
+  </si>
+  <si>
+    <t>Looping lobby/intro music</t>
+  </si>
+  <si>
+    <t>http://soundimage.org/wp-content/uploads/2016/06/Good-Morning-Doctor-Weird.mp3</t>
   </si>
 </sst>
 </file>
@@ -441,13 +465,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861FC0A8-580E-407C-B918-27B2E7524EEA}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="56.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="32.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -503,6 +532,48 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
One of the last pushes! I changed the readme to acknowledge third party assets
</commit_message>
<xml_diff>
--- a/public/mangos_game/Assets.xlsx
+++ b/public/mangos_game/Assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\CS5\git repository\public\mangos_game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C5B550-0AFE-4C6B-BB16-E36582C0427B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771343DA-1A49-4167-9DBA-8B7BF99B6E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="1410" windowWidth="14400" windowHeight="7360" xr2:uid="{7E3EC852-6885-4E01-BA36-ECA6C0A8927D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7E3EC852-6885-4E01-BA36-ECA6C0A8927D}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>